<commit_message>
fixed issues with excel save
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,24 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Session ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex</t>
+    <t xml:space="preserve">Participant Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
   </si>
   <si>
     <t xml:space="preserve">Normal Vision</t>
   </si>
   <si>
     <t xml:space="preserve">Colour Blind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaming hours</t>
   </si>
   <si>
     <t xml:space="preserve">Passive Block</t>
@@ -217,6 +223,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,27 +251,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,22 +276,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9433198380567"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -319,185 +325,202 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="15"/>
+      <c r="C15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="13"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="13"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="13"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="15"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="15"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
improved excel data logging
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t xml:space="preserve">Session ID</t>
   </si>
@@ -52,10 +52,100 @@
     <t xml:space="preserve">Trial</t>
   </si>
   <si>
+    <t xml:space="preserve">Trial type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q1: Was the behaviour normal?</t>
   </si>
   <si>
     <t xml:space="preserve">Q2: Mal or Faulty?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experiment Trial order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Healthy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 faulty sensors. 50% intermittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 faulty sensors. 50% intermittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 faulty sensors. 50% intermittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 malicious blockers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 malicious blockers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 malicious blockers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 malicious broadcaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 malicious broadcaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 faulty motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 faulty motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 faulty motors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active Block</t>
   </si>
 </sst>
 </file>
@@ -97,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -156,15 +246,22 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right/>
       <top style="hair"/>
-      <bottom style="hair"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair"/>
-      <top style="hair"/>
+      <right/>
+      <top/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
@@ -194,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,19 +340,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,22 +393,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:H51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5222672064777"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4372469635628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -370,157 +487,385 @@
       <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="E15" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="9"/>
       <c r="G16" s="8"/>
       <c r="H16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="15"/>
+      <c r="B17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="9"/>
       <c r="G17" s="8"/>
       <c r="H17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="15"/>
+      <c r="B18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="15"/>
+      <c r="B19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="9"/>
       <c r="G19" s="8"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="15"/>
+      <c r="B20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="9"/>
       <c r="G20" s="8"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="15"/>
+      <c r="B21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="15"/>
+      <c r="B22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="9"/>
       <c r="G22" s="8"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="15"/>
+      <c r="B23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="9"/>
       <c r="G23" s="8"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="15"/>
+      <c r="B24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="15"/>
+      <c r="B25" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="15"/>
+      <c r="B26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="15"/>
+      <c r="B27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+      <c r="B28" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+      <c r="B29" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
+      <c r="B32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
+      <c r="B33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
+      <c r="B34" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
+      <c r="B35" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
+      <c r="B36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="15"/>
+      <c r="B37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
+      <c r="B38" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
+      <c r="B39" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="18"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="18"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>